<commit_message>
updated data for 1/26
</commit_message>
<xml_diff>
--- a/virus.xlsx
+++ b/virus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\向菁\virus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0E4B5D-3C2A-47B2-997B-BEC6F2ACF1EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D9F520-E4E6-479B-9256-965A2EE8DD76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -74,7 +74,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,6 +607,17 @@
         <v>2058</v>
       </c>
     </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>43856</v>
+      </c>
+      <c r="B28">
+        <v>2583</v>
+      </c>
+      <c r="C28">
+        <v>2984</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add SIR model in the end, but it is not possible to try to apply it on current study
</commit_message>
<xml_diff>
--- a/virus.xlsx
+++ b/virus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\向菁\virus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D9F520-E4E6-479B-9256-965A2EE8DD76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D971A006-6DA7-4EDD-A834-4C4E69C90241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -355,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,7 +601,7 @@
         <v>43855</v>
       </c>
       <c r="B27">
-        <v>1412</v>
+        <v>2100</v>
       </c>
       <c r="C27">
         <v>2058</v>
@@ -612,10 +612,21 @@
         <v>43856</v>
       </c>
       <c r="B28">
-        <v>2583</v>
+        <v>2744</v>
       </c>
       <c r="C28">
-        <v>2984</v>
+        <v>5794</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>43857</v>
+      </c>
+      <c r="B29">
+        <v>4515</v>
+      </c>
+      <c r="C29">
+        <v>6973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data from NHC, add single point estimate according to suspected number
</commit_message>
<xml_diff>
--- a/virus.xlsx
+++ b/virus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\向菁\virus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D971A006-6DA7-4EDD-A834-4C4E69C90241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F65556-A4A6-4152-A5C2-C51BEF995271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,6 +81,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -100,7 +168,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -358,7 +426,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,7 +587,7 @@
         <v>43847</v>
       </c>
       <c r="B19">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -527,7 +595,7 @@
         <v>43848</v>
       </c>
       <c r="B20">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -535,7 +603,7 @@
         <v>43849</v>
       </c>
       <c r="B21">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C21">
         <v>40</v>
@@ -546,7 +614,7 @@
         <v>43850</v>
       </c>
       <c r="B22">
-        <v>258</v>
+        <v>291</v>
       </c>
       <c r="C22">
         <v>127</v>
@@ -557,7 +625,7 @@
         <v>43851</v>
       </c>
       <c r="B23">
-        <v>475</v>
+        <v>440</v>
       </c>
       <c r="C23">
         <v>260</v>
@@ -568,10 +636,10 @@
         <v>43852</v>
       </c>
       <c r="B24">
-        <v>522</v>
+        <v>571</v>
       </c>
       <c r="C24">
-        <v>330</v>
+        <v>393</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -579,10 +647,10 @@
         <v>43853</v>
       </c>
       <c r="B25">
-        <v>680</v>
+        <v>830</v>
       </c>
       <c r="C25">
-        <v>450</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -590,10 +658,10 @@
         <v>43854</v>
       </c>
       <c r="B26">
-        <v>1103</v>
+        <v>1287</v>
       </c>
       <c r="C26">
-        <v>1056</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -601,10 +669,10 @@
         <v>43855</v>
       </c>
       <c r="B27">
-        <v>2100</v>
+        <v>1975</v>
       </c>
       <c r="C27">
-        <v>2058</v>
+        <v>2684</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>